<commit_message>
Full recalculation with bug fixes
</commit_message>
<xml_diff>
--- a/python/results/tuning_summary.xlsx
+++ b/python/results/tuning_summary.xlsx
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="125">
   <si>
     <t>setup</t>
   </si>
@@ -316,18 +316,6 @@
     <t>alpha=0.223801135944, l1_ratio=0.8</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>gamma=0.01, lambda=2.0</t>
-  </si>
-  <si>
-    <t>gamma=1.0, lambda=3.0</t>
-  </si>
-  <si>
-    <t>gamma=0.1, lambda=2.0</t>
-  </si>
-  <si>
     <t>lambda 1=10.0, lambda 2=10.0</t>
   </si>
   <si>
@@ -364,15 +352,6 @@
     <t>alpha=0.413583525596, l1_ratio=0.1</t>
   </si>
   <si>
-    <t>gamma=1.0, lambda=2.0</t>
-  </si>
-  <si>
-    <t>gamma=100.0, lambda=2.0</t>
-  </si>
-  <si>
-    <t>gamma=10.0, lambda=2.0</t>
-  </si>
-  <si>
     <t>lambda 1=100.0, lambda 2=10.0</t>
   </si>
   <si>
@@ -487,12 +466,6 @@
     <t>alpha=0.367401981896, l1_ratio=0.1</t>
   </si>
   <si>
-    <t>gamma=10.0, lambda=3.0</t>
-  </si>
-  <si>
-    <t>gamma=0.01, lambda=3.0</t>
-  </si>
-  <si>
     <t>alpha=0.103587568802</t>
   </si>
   <si>
@@ -506,6 +479,30 @@
   </si>
   <si>
     <t>C=10.0</t>
+  </si>
+  <si>
+    <t>gamma=2.0, lambda=0.01</t>
+  </si>
+  <si>
+    <t>gamma=3.0, lambda=1.0</t>
+  </si>
+  <si>
+    <t>gamma=2.0, lambda=0.1</t>
+  </si>
+  <si>
+    <t>gamma=2.0, lambda=1.0</t>
+  </si>
+  <si>
+    <t>gamma=2.0, lambda=100.0</t>
+  </si>
+  <si>
+    <t>gamma=2.0, lambda=10.0</t>
+  </si>
+  <si>
+    <t>gamma=3.0, lambda=10.0</t>
+  </si>
+  <si>
+    <t>gamma=3.0, lambda=0.01</t>
   </si>
 </sst>
 </file>
@@ -2502,25 +2499,25 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>871.69055653199996</v>
+        <v>735.70405802799996</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>0.79888431673600002</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2534,7 +2531,7 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>218.73837657000001</v>
+        <v>218.74685539699999</v>
       </c>
       <c r="E7">
         <v>220</v>
@@ -2552,7 +2549,7 @@
         <v>0.2</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2566,25 +2563,25 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>341.43772960899997</v>
+        <v>259.93431759200001</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
+        <v>220</v>
+      </c>
+      <c r="F8">
+        <v>0.60917498607499998</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.109090909091</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2598,7 +2595,7 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>127.780421061</v>
+        <v>127.744039133</v>
       </c>
       <c r="E9">
         <v>220</v>
@@ -2616,7 +2613,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2648,7 +2645,7 @@
         <v>0.2</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2662,13 +2659,13 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>26.3193508974</v>
+        <v>20.8835301479</v>
       </c>
       <c r="E11">
         <v>220</v>
       </c>
       <c r="F11">
-        <v>0.80598233855300006</v>
+        <v>0.85788632569500001</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2680,7 +2677,7 @@
         <v>0.2</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2694,13 +2691,13 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>2.6077125831300001</v>
+        <v>5.6610267303799997</v>
       </c>
       <c r="E12">
         <v>220</v>
       </c>
       <c r="F12">
-        <v>0.87230977002599996</v>
+        <v>0.93250994180299995</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2712,7 +2709,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2726,13 +2723,13 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>5.28330629483</v>
+        <v>6.4996436722500004</v>
       </c>
       <c r="E13">
         <v>220</v>
       </c>
       <c r="F13">
-        <v>0.73884561142799998</v>
+        <v>0.79555144053500004</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2744,7 +2741,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2776,7 +2773,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2808,7 +2805,7 @@
         <v>0.60416666666700003</v>
       </c>
       <c r="J15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2840,7 +2837,7 @@
         <v>0.193181818182</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2872,7 +2869,7 @@
         <v>0.35897435897399999</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2936,7 +2933,7 @@
         <v>0.2</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3000,7 +2997,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3082,7 +3079,7 @@
         <v>0.25730994151999997</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3114,7 +3111,7 @@
         <v>0.23976608187099999</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3146,7 +3143,7 @@
         <v>0.15894039735099999</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3178,7 +3175,7 @@
         <v>0.14012738853500001</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3192,7 +3189,7 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>735.65313080800001</v>
+        <v>735.66811349199997</v>
       </c>
       <c r="E6">
         <v>220</v>
@@ -3210,7 +3207,7 @@
         <v>0.2</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3224,7 +3221,7 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>218.756911065</v>
+        <v>219.87200418200001</v>
       </c>
       <c r="E7">
         <v>220</v>
@@ -3242,7 +3239,7 @@
         <v>0.2</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3256,25 +3253,25 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>341.43772960899997</v>
+        <v>259.93689843099997</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
+        <v>220</v>
+      </c>
+      <c r="F8">
+        <v>0.60917498607499998</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.109090909091</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3288,7 +3285,7 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>127.799364248</v>
+        <v>128.074853512</v>
       </c>
       <c r="E9">
         <v>220</v>
@@ -3306,7 +3303,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3320,13 +3317,13 @@
         <v>36</v>
       </c>
       <c r="D10">
-        <v>5.0235583515300002</v>
+        <v>0.71469296498400003</v>
       </c>
       <c r="E10">
         <v>220</v>
       </c>
       <c r="F10">
-        <v>0.98987844280600001</v>
+        <v>0.99972646635700002</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3338,7 +3335,7 @@
         <v>0.2</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3352,13 +3349,13 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>26.3193508974</v>
+        <v>20.8835301479</v>
       </c>
       <c r="E11">
         <v>220</v>
       </c>
       <c r="F11">
-        <v>0.80598233855300006</v>
+        <v>0.85788632569500001</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3370,7 +3367,7 @@
         <v>0.2</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3402,7 +3399,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3434,7 +3431,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3466,7 +3463,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3498,7 +3495,7 @@
         <v>0.543859649123</v>
       </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3530,7 +3527,7 @@
         <v>0.53846153846199996</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3562,7 +3559,7 @@
         <v>0.34042553191500002</v>
       </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3576,7 +3573,7 @@
         <v>43</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3608,7 +3605,7 @@
         <v>0.2</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3640,7 +3637,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3672,7 +3669,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3883,7 +3880,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3947,7 +3944,7 @@
         <v>0.22857142857099999</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3979,7 +3976,7 @@
         <v>0.224299065421</v>
       </c>
       <c r="J9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4139,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4267,7 +4264,7 @@
         <v>0.59459459459499997</v>
       </c>
       <c r="J18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -4299,7 +4296,7 @@
         <v>0.27450980392199997</v>
       </c>
       <c r="J19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -4331,7 +4328,7 @@
         <v>0.25862068965500001</v>
       </c>
       <c r="J20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -4363,7 +4360,7 @@
         <v>0.13131313131299999</v>
       </c>
       <c r="J21" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -4395,7 +4392,7 @@
         <v>0.08</v>
       </c>
       <c r="J22" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -4427,7 +4424,7 @@
         <v>0.08</v>
       </c>
       <c r="J23" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -4459,7 +4456,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -4491,7 +4488,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J25" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -4651,7 +4648,7 @@
         <v>0.511627906977</v>
       </c>
       <c r="J30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -4683,7 +4680,7 @@
         <v>0.271844660194</v>
       </c>
       <c r="J31" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -4715,7 +4712,7 @@
         <v>0.26415094339599998</v>
       </c>
       <c r="J32" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4747,7 +4744,7 @@
         <v>0.13402061855700001</v>
       </c>
       <c r="J33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -4843,7 +4840,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4875,7 +4872,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4907,7 +4904,7 @@
         <v>0.08</v>
       </c>
       <c r="J38" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4939,7 +4936,7 @@
         <v>0.08</v>
       </c>
       <c r="J39" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4971,7 +4968,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J40" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -5003,7 +5000,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J41" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -5035,7 +5032,7 @@
         <v>0.08</v>
       </c>
       <c r="J42" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -5067,7 +5064,7 @@
         <v>0.08</v>
       </c>
       <c r="J43" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -5099,7 +5096,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -5131,7 +5128,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J45" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5213,7 +5210,7 @@
         <v>0.511627906977</v>
       </c>
       <c r="J2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5245,7 +5242,7 @@
         <v>0.41666666666699997</v>
       </c>
       <c r="J3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5277,7 +5274,7 @@
         <v>0.56666666666700005</v>
       </c>
       <c r="J4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5309,7 +5306,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5323,7 +5320,7 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>628.62396501499995</v>
+        <v>628.49356452300003</v>
       </c>
       <c r="E6">
         <v>550</v>
@@ -5341,7 +5338,7 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5355,7 +5352,7 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>224.73424633299999</v>
+        <v>224.88971647400001</v>
       </c>
       <c r="E7">
         <v>550</v>
@@ -5373,7 +5370,7 @@
         <v>0.08</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5387,25 +5384,25 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>312.91377539400003</v>
+        <v>247.705282098</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
+        <v>550</v>
+      </c>
+      <c r="F8">
+        <v>0.53759075755700003</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>4.36363636364E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5419,25 +5416,25 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>199.52836678599999</v>
+        <v>144.97737970200001</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
+        <v>550</v>
+      </c>
+      <c r="F9">
+        <v>0.43070704542400001</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>4.36363636364E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5469,7 +5466,7 @@
         <v>0.08</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5483,13 +5480,13 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>28.816500122200001</v>
+        <v>12.663817033100001</v>
       </c>
       <c r="E11">
         <v>550</v>
       </c>
       <c r="F11">
-        <v>0.73250890922300005</v>
+        <v>0.870026834784</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -5501,7 +5498,7 @@
         <v>0.08</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5515,13 +5512,13 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>1.73225017373</v>
+        <v>3.98588507347</v>
       </c>
       <c r="E12">
         <v>550</v>
       </c>
       <c r="F12">
-        <v>0.874072965993</v>
+        <v>0.94668429935200005</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -5533,7 +5530,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5547,13 +5544,13 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>7.0731073423500002</v>
+        <v>4.6063338489700003</v>
       </c>
       <c r="E13">
         <v>550</v>
       </c>
       <c r="F13">
-        <v>0.73166860077600004</v>
+        <v>0.855000712444</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -5565,7 +5562,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5597,7 +5594,7 @@
         <v>0.46236559139799999</v>
       </c>
       <c r="J14" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5629,7 +5626,7 @@
         <v>0.45901639344299999</v>
       </c>
       <c r="J15" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5661,7 +5658,7 @@
         <v>0.433333333333</v>
       </c>
       <c r="J16" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5693,7 +5690,7 @@
         <v>0.210526315789</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5757,7 +5754,7 @@
         <v>0.08</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5789,7 +5786,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5821,7 +5818,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -5905,7 +5902,7 @@
         <v>0.109181141439</v>
       </c>
       <c r="J2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5937,7 +5934,7 @@
         <v>0.12359550561800001</v>
       </c>
       <c r="J3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5969,7 +5966,7 @@
         <v>7.5709779179799999E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6001,7 +5998,7 @@
         <v>6.70926517572E-2</v>
       </c>
       <c r="J5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6015,7 +6012,7 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>628.59959798299997</v>
+        <v>628.473183027</v>
       </c>
       <c r="E6">
         <v>550</v>
@@ -6033,7 +6030,7 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -6047,25 +6044,25 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>279.53681389100001</v>
+        <v>224.68550315600001</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
+        <v>550</v>
+      </c>
+      <c r="F7">
+        <v>0.45698462269599999</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -6079,25 +6076,25 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>312.91377539400003</v>
+        <v>247.70438373299999</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
+        <v>550</v>
+      </c>
+      <c r="F8">
+        <v>0.53759075755700003</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>4.36363636364E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -6111,25 +6108,25 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>199.52836678599999</v>
+        <v>144.979623917</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
+        <v>550</v>
+      </c>
+      <c r="F9">
+        <v>0.43070704542400001</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>4.36363636364E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -6143,13 +6140,13 @@
         <v>36</v>
       </c>
       <c r="D10">
-        <v>3.2448863638600001</v>
+        <v>0.33140450417599998</v>
       </c>
       <c r="E10">
         <v>550</v>
       </c>
       <c r="F10">
-        <v>0.98899279809600005</v>
+        <v>0.99988324791100003</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -6161,7 +6158,7 @@
         <v>0.08</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -6175,13 +6172,13 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>28.816500122200001</v>
+        <v>12.663817033100001</v>
       </c>
       <c r="E11">
         <v>550</v>
       </c>
       <c r="F11">
-        <v>0.73250890922300005</v>
+        <v>0.870026834784</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -6193,7 +6190,7 @@
         <v>0.08</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -6225,7 +6222,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -6257,7 +6254,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -6289,7 +6286,7 @@
         <v>0.46236559139799999</v>
       </c>
       <c r="J14" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -6321,7 +6318,7 @@
         <v>0.33750000000000002</v>
       </c>
       <c r="J15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -6353,7 +6350,7 @@
         <v>0.16483516483499999</v>
       </c>
       <c r="J16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -6385,7 +6382,7 @@
         <v>0.19354838709700001</v>
       </c>
       <c r="J17" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6417,7 +6414,7 @@
         <v>0.08</v>
       </c>
       <c r="J18" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -6449,7 +6446,7 @@
         <v>0.08</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -6463,7 +6460,7 @@
         <v>43</v>
       </c>
       <c r="J20" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -6495,7 +6492,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated optimal values before recalc
</commit_message>
<xml_diff>
--- a/python/results/tuning_summary.xlsx
+++ b/python/results/tuning_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cv_mse_p220" sheetId="1" r:id="rId1"/>
@@ -3515,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Tuning with latest solver settings
</commit_message>
<xml_diff>
--- a/python/results/tuning_summary.xlsx
+++ b/python/results/tuning_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cv_mse_p220" sheetId="1" r:id="rId1"/>
@@ -208,36 +208,9 @@
     <t>ttlp</t>
   </si>
   <si>
-    <t>alpha=0.0345473635982, l1_ratio=0.8</t>
-  </si>
-  <si>
-    <t>alpha=0.511689891439, l1_ratio=0.9</t>
-  </si>
-  <si>
-    <t>alpha=0.369439795992, l1_ratio=0.9</t>
-  </si>
-  <si>
-    <t>alpha=0.223801135944, l1_ratio=0.8</t>
-  </si>
-  <si>
-    <t>lambda 1=10.0, lambda 2=10.0</t>
-  </si>
-  <si>
     <t>lambda 1=10.0, lambda 2=100.0</t>
   </si>
   <si>
-    <t>alpha=0.0301862495166</t>
-  </si>
-  <si>
-    <t>alpha=0.313968172661</t>
-  </si>
-  <si>
-    <t>alpha=0.0145840029776</t>
-  </si>
-  <si>
-    <t>alpha=0.209681233894</t>
-  </si>
-  <si>
     <t>C=35.0</t>
   </si>
   <si>
@@ -253,12 +226,6 @@
     <t>alpha=0.413583525596, l1_ratio=0.1</t>
   </si>
   <si>
-    <t>lambda 1=100.0, lambda 2=10.0</t>
-  </si>
-  <si>
-    <t>alpha=0.192647959425</t>
-  </si>
-  <si>
     <t>alpha=0.254859593892</t>
   </si>
   <si>
@@ -268,24 +235,9 @@
     <t>E=70.0</t>
   </si>
   <si>
-    <t>alpha=0.0215751505702, l1_ratio=0.9</t>
-  </si>
-  <si>
-    <t>alpha=0.635296423133, l1_ratio=0.9</t>
-  </si>
-  <si>
-    <t>alpha=0.263021624619, l1_ratio=0.9</t>
-  </si>
-  <si>
     <t>alpha=0.0181089518682</t>
   </si>
   <si>
-    <t>alpha=0.121263561278</t>
-  </si>
-  <si>
-    <t>alpha=0.159773753657</t>
-  </si>
-  <si>
     <t>alpha=1.04672808601, l1_ratio=0.1</t>
   </si>
   <si>
@@ -307,21 +259,12 @@
     <t>gamma=2.0, lambda=0.01</t>
   </si>
   <si>
-    <t>gamma=3.0, lambda=1.0</t>
-  </si>
-  <si>
     <t>gamma=2.0, lambda=0.1</t>
   </si>
   <si>
     <t>gamma=2.0, lambda=1.0</t>
   </si>
   <si>
-    <t>gamma=2.0, lambda=10.0</t>
-  </si>
-  <si>
-    <t>gamma=3.0, lambda=10.0</t>
-  </si>
-  <si>
     <t>gamma=3.0, lambda=0.01</t>
   </si>
   <si>
@@ -400,15 +343,9 @@
     <t>tau=2.99870761465, delta 1=415.32100463, delta 2=5.99741522931</t>
   </si>
   <si>
-    <t>alpha=0.42205481678, l1_ratio=0.9</t>
-  </si>
-  <si>
     <t>gamma=2.0, lambda=1000.0</t>
   </si>
   <si>
-    <t>alpha=0.256594317455</t>
-  </si>
-  <si>
     <t>gamma=3.0, lambda=100.0</t>
   </si>
   <si>
@@ -424,9 +361,6 @@
     <t>alpha=0.112717224649</t>
   </si>
   <si>
-    <t>C=60.0</t>
-  </si>
-  <si>
     <t>E=15.0</t>
   </si>
   <si>
@@ -478,10 +412,76 @@
     <t>gamma=3.0, lambda=0.1</t>
   </si>
   <si>
-    <t>alpha=0.552963768506, l1_ratio=0.1</t>
-  </si>
-  <si>
-    <t>C=25.0</t>
+    <t>alpha=0.016272215615, l1_ratio=0.7</t>
+  </si>
+  <si>
+    <t>alpha=0.0151010363257, l1_ratio=0.7</t>
+  </si>
+  <si>
+    <t>alpha=0.229693860143, l1_ratio=0.9</t>
+  </si>
+  <si>
+    <t>alpha=0.0130448555261, l1_ratio=0.4</t>
+  </si>
+  <si>
+    <t>lambda 1=10.0, lambda 2=1.0</t>
+  </si>
+  <si>
+    <t>lambda 1=1.0, lambda 2=1.0</t>
+  </si>
+  <si>
+    <t>alpha=0.0161094934588</t>
+  </si>
+  <si>
+    <t>alpha=0.0126749493168</t>
+  </si>
+  <si>
+    <t>alpha=0.012684422044</t>
+  </si>
+  <si>
+    <t>alpha=0.0846486760032</t>
+  </si>
+  <si>
+    <t>C=45.0</t>
+  </si>
+  <si>
+    <t>alpha=0.461163829722, l1_ratio=0.1</t>
+  </si>
+  <si>
+    <t>lambda 1=1.0, lambda 2=0.1</t>
+  </si>
+  <si>
+    <t>alpha=0.0511689891439</t>
+  </si>
+  <si>
+    <t>C=40.0</t>
+  </si>
+  <si>
+    <t>alpha=0.0487681926312, l1_ratio=0.8</t>
+  </si>
+  <si>
+    <t>alpha=0.055714363846, l1_ratio=0.9</t>
+  </si>
+  <si>
+    <t>alpha=0.333754556095, l1_ratio=0.8</t>
+  </si>
+  <si>
+    <t>alpha=0.0213344948893, l1_ratio=0.5</t>
+  </si>
+  <si>
+    <t>alpha=0.0223255622654</t>
+  </si>
+  <si>
+    <t>alpha=0.0840230707421</t>
+  </si>
+  <si>
+    <t>alpha=0.120862985347</t>
+  </si>
+  <si>
+    <t>C=100.0</t>
+  </si>
+  <si>
+    <t>C=65.0</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
         <v>0.63768115942000003</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -943,7 +943,7 @@
         <v>0.448275862069</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -975,7 +975,7 @@
         <v>0.28301886792499997</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1007,7 +1007,7 @@
         <v>0.26388888888899997</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1021,7 +1021,7 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1053,7 +1053,7 @@
         <v>0.2</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1085,7 +1085,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1117,7 +1117,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J9" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1128,7 +1128,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>2.8094266887199999</v>
@@ -1149,7 +1149,7 @@
         <v>0.62857142857100001</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1160,7 +1160,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>20.879828996200001</v>
@@ -1181,7 +1181,7 @@
         <v>0.35714285714299998</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1192,7 +1192,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>0.96556700412499996</v>
@@ -1213,7 +1213,7 @@
         <v>0.28301886792499997</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1224,7 +1224,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>10.4076367667</v>
@@ -1245,7 +1245,7 @@
         <v>0.20618556700999999</v>
       </c>
       <c r="J13" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1309,7 +1309,7 @@
         <v>0.39583333333300003</v>
       </c>
       <c r="J15" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1341,7 +1341,7 @@
         <v>0.26315789473700002</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1387,13 +1387,13 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>735.70405802799996</v>
+        <v>381.33024746000001</v>
       </c>
       <c r="E18">
         <v>220</v>
       </c>
       <c r="F18">
-        <v>0.79888431673600002</v>
+        <v>0.84776209211999998</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1405,7 +1405,7 @@
         <v>0.2</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1419,13 +1419,13 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>218.74685539699999</v>
+        <v>126.740249361</v>
       </c>
       <c r="E19">
         <v>220</v>
       </c>
       <c r="F19">
-        <v>0.48853167543499998</v>
+        <v>0.54859258023500002</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>0.2</v>
       </c>
       <c r="J19" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1451,13 +1451,13 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>259.63641981799998</v>
+        <v>129.28163286</v>
       </c>
       <c r="E20">
         <v>220</v>
       </c>
       <c r="F20">
-        <v>0.60917498607499998</v>
+        <v>0.62010159906700002</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1469,7 +1469,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1483,13 +1483,13 @@
         <v>18</v>
       </c>
       <c r="D21">
-        <v>128.12177284800001</v>
+        <v>57.169596288100003</v>
       </c>
       <c r="E21">
         <v>220</v>
       </c>
       <c r="F21">
-        <v>0.45783749396399998</v>
+        <v>0.50335334674599996</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1501,7 +1501,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J21" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1533,7 +1533,7 @@
         <v>0.29139072847699998</v>
       </c>
       <c r="J22" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1565,7 +1565,7 @@
         <v>0.37623762376199998</v>
       </c>
       <c r="J23" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1597,7 +1597,7 @@
         <v>0.28846153846200001</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1629,7 +1629,7 @@
         <v>0.26760563380300001</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1661,7 +1661,7 @@
         <v>0.619718309859</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1693,7 +1693,7 @@
         <v>0.40625</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1725,7 +1725,7 @@
         <v>0.25423728813599999</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1757,7 +1757,7 @@
         <v>0.218390804598</v>
       </c>
       <c r="J29" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1853,7 +1853,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J32" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1885,7 +1885,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J33" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1917,7 +1917,7 @@
         <v>0.2</v>
       </c>
       <c r="J34" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1949,7 +1949,7 @@
         <v>0.2</v>
       </c>
       <c r="J35" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1981,7 +1981,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J36" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2013,7 +2013,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J37" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2045,7 +2045,7 @@
         <v>0.2</v>
       </c>
       <c r="J38" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2077,7 +2077,7 @@
         <v>0.2</v>
       </c>
       <c r="J39" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2109,7 +2109,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J40" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2141,7 +2141,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J41" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2205,25 +2205,25 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>2.8078610745999999</v>
+        <v>3.4423618621699998</v>
       </c>
       <c r="E2">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F2">
-        <v>0.98467214998899999</v>
+        <v>0.97515105106699995</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.77840909090900001</v>
+        <v>0.6875</v>
       </c>
       <c r="I2">
-        <v>0.53012048192799999</v>
+        <v>0.444444444444</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2237,25 +2237,25 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>23.607529756600002</v>
+        <v>18.444014057</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="F3">
-        <v>0.79776360147699998</v>
+        <v>0.77381993047499997</v>
       </c>
       <c r="G3">
-        <v>0.68181818181800002</v>
+        <v>0.84090909090900001</v>
       </c>
       <c r="H3">
-        <v>0.94318181818199998</v>
+        <v>0.55681818181800002</v>
       </c>
       <c r="I3">
-        <v>0.75</v>
+        <v>0.32173913043500002</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2269,25 +2269,25 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>3.52989199754</v>
+        <v>1.9675326366799999</v>
       </c>
       <c r="E4">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F4">
-        <v>0.97621442782500001</v>
+        <v>0.98656096061200005</v>
       </c>
       <c r="G4">
-        <v>0.75</v>
+        <v>0.70833333333299997</v>
       </c>
       <c r="H4">
-        <v>0.92346938775499998</v>
+        <v>0.90306122449000004</v>
       </c>
       <c r="I4">
-        <v>0.54545454545500005</v>
+        <v>0.472222222222</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2301,25 +2301,25 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>5.1694122649500001</v>
+        <v>9.1227559600700001</v>
       </c>
       <c r="E5">
-        <v>56</v>
+        <v>139</v>
       </c>
       <c r="F5">
-        <v>0.81274229821999999</v>
+        <v>0.717897624904</v>
       </c>
       <c r="G5">
-        <v>0.75</v>
+        <v>0.91666666666700003</v>
       </c>
       <c r="H5">
-        <v>0.80612244897999996</v>
+        <v>0.40306122448999998</v>
       </c>
       <c r="I5">
-        <v>0.321428571429</v>
+        <v>0.15827338129499999</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2333,13 +2333,13 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>735.70031429200003</v>
+        <v>291.062271963</v>
       </c>
       <c r="E6">
         <v>220</v>
       </c>
       <c r="F6">
-        <v>0.79888431673600002</v>
+        <v>0.58258507012600003</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2351,7 +2351,7 @@
         <v>0.2</v>
       </c>
       <c r="J6" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2365,13 +2365,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>218.74685539699999</v>
+        <v>127.63119459399999</v>
       </c>
       <c r="E7">
         <v>220</v>
       </c>
       <c r="F7">
-        <v>0.48853167543499998</v>
+        <v>0.54776609538400001</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -2383,7 +2383,7 @@
         <v>0.2</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2397,13 +2397,13 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>259.93396609799998</v>
+        <v>126.528047704</v>
       </c>
       <c r="E8">
         <v>220</v>
       </c>
       <c r="F8">
-        <v>0.60917498607499998</v>
+        <v>0.468312914011</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -2415,7 +2415,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J8" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2429,13 +2429,13 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>127.707023091</v>
+        <v>53.916244665199997</v>
       </c>
       <c r="E9">
         <v>220</v>
       </c>
       <c r="F9">
-        <v>0.45783749396399998</v>
+        <v>0.49725969477300003</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2447,7 +2447,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2461,25 +2461,25 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>1.0411899150499999</v>
+        <v>0.99640395367699996</v>
       </c>
       <c r="E10">
+        <v>165</v>
+      </c>
+      <c r="F10">
+        <v>0.99775422064599995</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.3125</v>
+      </c>
+      <c r="I10">
+        <v>0.26666666666700001</v>
+      </c>
+      <c r="J10" t="s">
         <v>73</v>
-      </c>
-      <c r="F10">
-        <v>0.99783430678499996</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0.83522727272700004</v>
-      </c>
-      <c r="I10">
-        <v>0.60273972602699999</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2493,25 +2493,25 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>20.883530251700002</v>
+        <v>13.824991992199999</v>
       </c>
       <c r="E11">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="F11">
-        <v>0.85788632559099998</v>
+        <v>0.87048882788000004</v>
       </c>
       <c r="G11">
-        <v>0.68181818181800002</v>
+        <v>0.86363636363600005</v>
       </c>
       <c r="H11">
-        <v>0.94886363636399995</v>
+        <v>0.65909090909099999</v>
       </c>
       <c r="I11">
-        <v>0.76923076923099998</v>
+        <v>0.387755102041</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2525,25 +2525,25 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>5.6610269002600004</v>
+        <v>3.5570468120699998</v>
       </c>
       <c r="E12">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="F12">
-        <v>0.932509941826</v>
+        <v>0.89899513665300002</v>
       </c>
       <c r="G12">
-        <v>0.91666666666700003</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0.92346938775499998</v>
+        <v>0.46938775510199998</v>
       </c>
       <c r="I12">
-        <v>0.59459459459499997</v>
+        <v>0.1875</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2557,25 +2557,25 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>6.4996438538600003</v>
+        <v>6.8742040207199997</v>
       </c>
       <c r="E13">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="F13">
-        <v>0.79555144054600002</v>
+        <v>0.76542797706700005</v>
       </c>
       <c r="G13">
-        <v>0.70833333333299997</v>
+        <v>0.91666666666700003</v>
       </c>
       <c r="H13">
-        <v>0.92857142857099995</v>
+        <v>0.41326530612200002</v>
       </c>
       <c r="I13">
-        <v>0.54838709677399999</v>
+        <v>0.16058394160600001</v>
       </c>
       <c r="J13" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2589,25 +2589,25 @@
         <v>20</v>
       </c>
       <c r="D14">
-        <v>2.4226923936000002</v>
+        <v>3.14108498528</v>
       </c>
       <c r="E14">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F14">
-        <v>0.98876556649900005</v>
+        <v>0.98419767352400001</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.79545454545500005</v>
+        <v>0.73863636363600005</v>
       </c>
       <c r="I14">
-        <v>0.55000000000000004</v>
+        <v>0.48888888888900001</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2621,25 +2621,25 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>23.848641473099999</v>
+        <v>15.2047464685</v>
       </c>
       <c r="E15">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="F15">
-        <v>0.76681852188800004</v>
+        <v>0.846159682503</v>
       </c>
       <c r="G15">
-        <v>0.65909090909099999</v>
+        <v>0.88636363636399995</v>
       </c>
       <c r="H15">
-        <v>0.89204545454499995</v>
+        <v>0.67045454545500005</v>
       </c>
       <c r="I15">
-        <v>0.60416666666700003</v>
+        <v>0.40206185567000002</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2653,25 +2653,25 @@
         <v>20</v>
       </c>
       <c r="D16">
-        <v>1.01686023535</v>
+        <v>1.0401728343000001</v>
       </c>
       <c r="E16">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F16">
-        <v>0.99611942424800004</v>
+        <v>0.995908775084</v>
       </c>
       <c r="G16">
         <v>0.70833333333299997</v>
       </c>
       <c r="H16">
-        <v>0.63775510204100005</v>
+        <v>0.617346938776</v>
       </c>
       <c r="I16">
-        <v>0.193181818182</v>
+        <v>0.18478260869599999</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2685,25 +2685,25 @@
         <v>20</v>
       </c>
       <c r="D17">
-        <v>5.8846780675700003</v>
+        <v>4.6328581183699997</v>
       </c>
       <c r="E17">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F17">
-        <v>0.80662708194199995</v>
+        <v>0.87306609334200003</v>
       </c>
       <c r="G17">
-        <v>0.58333333333299997</v>
+        <v>0.79166666666700003</v>
       </c>
       <c r="H17">
-        <v>0.87244897959199996</v>
+        <v>0.76020408163300002</v>
       </c>
       <c r="I17">
-        <v>0.35897435897399999</v>
+        <v>0.28787878787900001</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2717,13 +2717,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>1.6491242512299999</v>
+        <v>1.5740420695799999</v>
       </c>
       <c r="E18">
         <v>220</v>
       </c>
       <c r="F18">
-        <v>0.99212458743700005</v>
+        <v>0.99294789023100005</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2735,7 +2735,7 @@
         <v>0.2</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2749,13 +2749,13 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>21.281859357399998</v>
+        <v>5.6666493811900001</v>
       </c>
       <c r="E19">
         <v>220</v>
       </c>
       <c r="F19">
-        <v>0.80239214160899996</v>
+        <v>0.95797877475500004</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2767,7 +2767,7 @@
         <v>0.2</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2813,13 +2813,13 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>7.0504797826000001</v>
+        <v>7.6474174601299998</v>
       </c>
       <c r="E21">
         <v>220</v>
       </c>
       <c r="F21">
-        <v>0.74547686476399999</v>
+        <v>0.74835916254199997</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2831,7 +2831,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J21" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2913,7 +2913,7 @@
         <v>0.25730994151999997</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2927,25 +2927,25 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>39.496961729399999</v>
+        <v>38.0288181998</v>
       </c>
       <c r="E3">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F3">
-        <v>0.67368349458800003</v>
+        <v>0.675958504367</v>
       </c>
       <c r="G3">
-        <v>0.90909090909099999</v>
+        <v>0.93181818181800002</v>
       </c>
       <c r="H3">
-        <v>0.26704545454500001</v>
+        <v>0.26136363636400001</v>
       </c>
       <c r="I3">
-        <v>0.236686390533</v>
+        <v>0.23976608187099999</v>
       </c>
       <c r="J3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2977,7 +2977,7 @@
         <v>0.15894039735099999</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3009,7 +3009,7 @@
         <v>0.14012738853500001</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3023,13 +3023,13 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>735.70076644599999</v>
+        <v>291.062271963</v>
       </c>
       <c r="E6">
         <v>220</v>
       </c>
       <c r="F6">
-        <v>0.79888431673600002</v>
+        <v>0.58258507012600003</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3041,7 +3041,7 @@
         <v>0.2</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3055,13 +3055,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>218.74685539699999</v>
+        <v>127.63119459399999</v>
       </c>
       <c r="E7">
         <v>220</v>
       </c>
       <c r="F7">
-        <v>0.48853167543499998</v>
+        <v>0.54776609538400001</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -3073,7 +3073,7 @@
         <v>0.2</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3087,13 +3087,13 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>259.93431759200001</v>
+        <v>126.528047704</v>
       </c>
       <c r="E8">
         <v>220</v>
       </c>
       <c r="F8">
-        <v>0.60917498607499998</v>
+        <v>0.468312914011</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3105,7 +3105,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3119,13 +3119,13 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>127.707023091</v>
+        <v>53.916244665199997</v>
       </c>
       <c r="E9">
         <v>220</v>
       </c>
       <c r="F9">
-        <v>0.45783749396399998</v>
+        <v>0.49725969477300003</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3137,7 +3137,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3169,7 +3169,7 @@
         <v>0.44</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3183,25 +3183,25 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>17.869583560300001</v>
+        <v>13.5056305839</v>
       </c>
       <c r="E11">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="F11">
-        <v>0.85773751188900005</v>
+        <v>0.86125926927100005</v>
       </c>
       <c r="G11">
-        <v>0.86363636363600005</v>
+        <v>0.88636363636399995</v>
       </c>
       <c r="H11">
-        <v>0.48863636363599999</v>
+        <v>0.61363636363600005</v>
       </c>
       <c r="I11">
-        <v>0.296875</v>
+        <v>0.36448598130799997</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3233,7 +3233,7 @@
         <v>0.19672131147499999</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3265,7 +3265,7 @@
         <v>0.14285714285699999</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3279,25 +3279,25 @@
         <v>20</v>
       </c>
       <c r="D14">
-        <v>2.4226923936000002</v>
+        <v>3.14108498528</v>
       </c>
       <c r="E14">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F14">
-        <v>0.98876556649900005</v>
+        <v>0.98419767352400001</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.79545454545500005</v>
+        <v>0.73863636363600005</v>
       </c>
       <c r="I14">
-        <v>0.55000000000000004</v>
+        <v>0.48888888888900001</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3311,25 +3311,25 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>22.8064829602</v>
+        <v>14.883793239399999</v>
       </c>
       <c r="E15">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="F15">
-        <v>0.77357433533700004</v>
+        <v>0.83932749020599995</v>
       </c>
       <c r="G15">
-        <v>0.70454545454499995</v>
+        <v>0.88636363636399995</v>
       </c>
       <c r="H15">
-        <v>0.85227272727299996</v>
+        <v>0.71590909090900001</v>
       </c>
       <c r="I15">
-        <v>0.543859649123</v>
+        <v>0.43820224719099998</v>
       </c>
       <c r="J15" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3361,7 +3361,7 @@
         <v>0.53846153846199996</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3393,7 +3393,7 @@
         <v>0.34042553191500002</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3406,8 +3406,26 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
+      <c r="D18">
+        <v>1.6491242512299999</v>
+      </c>
+      <c r="E18">
+        <v>220</v>
+      </c>
+      <c r="F18">
+        <v>0.99212458743700005</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
       <c r="J18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3421,13 +3439,13 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>21.281859357399998</v>
+        <v>8.5503789009800002</v>
       </c>
       <c r="E19">
         <v>220</v>
       </c>
       <c r="F19">
-        <v>0.80239214160899996</v>
+        <v>0.92766278073800001</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3439,7 +3457,7 @@
         <v>0.2</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3453,13 +3471,13 @@
         <v>21</v>
       </c>
       <c r="D20">
-        <v>4.76501979861</v>
+        <v>4.7854142521399998</v>
       </c>
       <c r="E20">
         <v>220</v>
       </c>
       <c r="F20">
-        <v>0.83706254160899995</v>
+        <v>0.83563938396199999</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -3471,7 +3489,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3485,13 +3503,13 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>6.0136016397200001</v>
+        <v>7.0504797826000001</v>
       </c>
       <c r="E21">
         <v>220</v>
       </c>
       <c r="F21">
-        <v>0.72165248646199998</v>
+        <v>0.74547686476399999</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3503,7 +3521,7 @@
         <v>0.109090909091</v>
       </c>
       <c r="J21" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3515,7 +3533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3589,7 +3607,7 @@
         <v>0.56410256410299997</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3621,7 +3639,7 @@
         <v>0.31868131868100003</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3653,7 +3671,7 @@
         <v>0.3</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3685,7 +3703,7 @@
         <v>0.156626506024</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3717,7 +3735,7 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3749,7 +3767,7 @@
         <v>0.08</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3781,7 +3799,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3813,7 +3831,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3824,7 +3842,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>0.86377309511599998</v>
@@ -3845,7 +3863,7 @@
         <v>0.69841269841300002</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3856,7 +3874,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>18.189474905000001</v>
@@ -3877,7 +3895,7 @@
         <v>0.32954545454500001</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3888,7 +3906,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>0.28926720307100001</v>
@@ -3909,7 +3927,7 @@
         <v>0.3</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3920,7 +3938,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>6.2246364431299996</v>
@@ -3941,7 +3959,7 @@
         <v>0.139784946237</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3973,7 +3991,7 @@
         <v>0.58666666666699996</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4005,7 +4023,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -4037,7 +4055,7 @@
         <v>0.245901639344</v>
       </c>
       <c r="J16" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -4069,7 +4087,7 @@
         <v>0.13402061855700001</v>
       </c>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4083,13 +4101,13 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>628.473183027</v>
+        <v>341.85845749399999</v>
       </c>
       <c r="E18">
         <v>550</v>
       </c>
       <c r="F18">
-        <v>0.66857624268500004</v>
+        <v>0.58803433362500002</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -4101,7 +4119,7 @@
         <v>0.08</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -4115,13 +4133,13 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>224.88971647400001</v>
+        <v>102.903923116</v>
       </c>
       <c r="E19">
         <v>550</v>
       </c>
       <c r="F19">
-        <v>0.45698462269599999</v>
+        <v>0.401475686635</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -4133,7 +4151,7 @@
         <v>0.08</v>
       </c>
       <c r="J19" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -4147,13 +4165,13 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>247.62656841399999</v>
+        <v>139.59971904400001</v>
       </c>
       <c r="E20">
         <v>550</v>
       </c>
       <c r="F20">
-        <v>0.53759075755700003</v>
+        <v>0.48500251585600002</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -4165,7 +4183,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -4179,13 +4197,13 @@
         <v>18</v>
       </c>
       <c r="D21">
-        <v>144.73425902</v>
+        <v>95.458197283499999</v>
       </c>
       <c r="E21">
         <v>550</v>
       </c>
       <c r="F21">
-        <v>0.43070704542400001</v>
+        <v>0.40716759877300002</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -4197,7 +4215,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -4229,7 +4247,7 @@
         <v>0.196428571429</v>
       </c>
       <c r="J22" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -4261,7 +4279,7 @@
         <v>0.31868131868100003</v>
       </c>
       <c r="J23" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -4293,7 +4311,7 @@
         <v>0.26415094339599998</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -4325,7 +4343,7 @@
         <v>0.14141414141399999</v>
       </c>
       <c r="J25" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -4357,7 +4375,7 @@
         <v>0.51764705882399997</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -4389,7 +4407,7 @@
         <v>0.292929292929</v>
       </c>
       <c r="J27" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -4421,7 +4439,7 @@
         <v>0.25423728813599999</v>
       </c>
       <c r="J28" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -4453,7 +4471,7 @@
         <v>0.135416666667</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -4549,7 +4567,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J32" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4581,7 +4599,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J33" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -4613,7 +4631,7 @@
         <v>0.08</v>
       </c>
       <c r="J34" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -4645,7 +4663,7 @@
         <v>0.08</v>
       </c>
       <c r="J35" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4677,7 +4695,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J36" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4709,7 +4727,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J37" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4741,7 +4759,7 @@
         <v>0.08</v>
       </c>
       <c r="J38" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4773,7 +4791,7 @@
         <v>0.08</v>
       </c>
       <c r="J39" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4805,7 +4823,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J40" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -4837,7 +4855,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J41" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -4903,25 +4921,25 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>1.09543119051</v>
+        <v>1.4219133989299999</v>
       </c>
       <c r="E2">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F2">
-        <v>0.99360905096399998</v>
+        <v>0.990287828303</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.91699604743100005</v>
+        <v>0.92094861660100003</v>
       </c>
       <c r="I2">
-        <v>0.511627906977</v>
+        <v>0.52380952381000001</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4935,25 +4953,25 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>14.0188023991</v>
+        <v>15.7943687469</v>
       </c>
       <c r="E3">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="F3">
-        <v>0.82241121535499995</v>
+        <v>0.77417539301500005</v>
       </c>
       <c r="G3">
         <v>0.65909090909099999</v>
       </c>
       <c r="H3">
-        <v>0.94664031620599998</v>
+        <v>0.871541501976</v>
       </c>
       <c r="I3">
-        <v>0.51785714285700002</v>
+        <v>0.30851063829800002</v>
       </c>
       <c r="J3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4967,25 +4985,25 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>5.3399083446900004</v>
+        <v>2.8377520608000002</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F4">
-        <v>0.97024120869800001</v>
+        <v>0.95119039878099998</v>
       </c>
       <c r="G4">
-        <v>0.70833333333299997</v>
+        <v>0.95833333333299997</v>
       </c>
       <c r="H4">
-        <v>0.97528517110299995</v>
+        <v>0.95247148289000005</v>
       </c>
       <c r="I4">
-        <v>0.56666666666700005</v>
+        <v>0.47916666666699997</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4999,25 +5017,25 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>4.1737677492499996</v>
+        <v>9.3995017672400003</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="F5">
-        <v>0.86932222829000005</v>
+        <v>0.71554028327200003</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.70833333333299997</v>
       </c>
       <c r="H5">
-        <v>0.93155893536099998</v>
+        <v>0.77186311787100004</v>
       </c>
       <c r="I5">
-        <v>0.25</v>
+        <v>0.12408759124099999</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5031,13 +5049,13 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>628.67378185699999</v>
+        <v>343.82449292199999</v>
       </c>
       <c r="E6">
         <v>550</v>
       </c>
       <c r="F6">
-        <v>0.66857624268500004</v>
+        <v>0.58823110544500001</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -5049,7 +5067,7 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5063,13 +5081,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>267.87201670799999</v>
+        <v>132.271365008</v>
       </c>
       <c r="E7">
         <v>550</v>
       </c>
       <c r="F7">
-        <v>0.45698462269599999</v>
+        <v>0.46056804825199998</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -5081,7 +5099,7 @@
         <v>0.08</v>
       </c>
       <c r="J7" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5095,13 +5113,13 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>247.695633141</v>
+        <v>139.59971904400001</v>
       </c>
       <c r="E8">
         <v>550</v>
       </c>
       <c r="F8">
-        <v>0.53759075755700003</v>
+        <v>0.48500251585600002</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -5113,7 +5131,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5127,13 +5145,13 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>144.97965451300001</v>
+        <v>95.458197283499999</v>
       </c>
       <c r="E9">
         <v>550</v>
       </c>
       <c r="F9">
-        <v>0.43070704542400001</v>
+        <v>0.40716759877300002</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -5145,7 +5163,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5159,25 +5177,25 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>0.40173143925799998</v>
+        <v>0.331404494499</v>
       </c>
       <c r="E10">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="F10">
-        <v>0.99923057909799995</v>
+        <v>0.99988324791100003</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.93280632411099995</v>
+        <v>0.86363636363600005</v>
       </c>
       <c r="I10">
-        <v>0.56410256410299997</v>
+        <v>0.38938053097300002</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5191,25 +5209,25 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>12.6638172155</v>
+        <v>13.9135547624</v>
       </c>
       <c r="E11">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F11">
-        <v>0.87002683465099995</v>
+        <v>0.82236670105599996</v>
       </c>
       <c r="G11">
-        <v>0.68181818181800002</v>
+        <v>0.70454545454499995</v>
       </c>
       <c r="H11">
-        <v>0.95652173913000005</v>
+        <v>0.85968379446599996</v>
       </c>
       <c r="I11">
-        <v>0.57692307692300004</v>
+        <v>0.30392156862699998</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5223,25 +5241,25 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>3.9858850802300001</v>
+        <v>2.2362303237900001</v>
       </c>
       <c r="E12">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="F12">
-        <v>0.94668429935099996</v>
+        <v>0.89629574742600004</v>
       </c>
       <c r="G12">
-        <v>0.95833333333299997</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0.96577946768099998</v>
+        <v>0.75665399239499997</v>
       </c>
       <c r="I12">
-        <v>0.56097560975600003</v>
+        <v>0.15789473684200001</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5255,25 +5273,25 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>4.6063342244100003</v>
+        <v>7.2083433832599999</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="F13">
-        <v>0.85500071247200005</v>
+        <v>0.76443512238199995</v>
       </c>
       <c r="G13">
-        <v>0.54166666666700003</v>
+        <v>0.83333333333299997</v>
       </c>
       <c r="H13">
-        <v>0.96768060836500003</v>
+        <v>0.73193916349800003</v>
       </c>
       <c r="I13">
-        <v>0.433333333333</v>
+        <v>0.124223602484</v>
       </c>
       <c r="J13" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5287,25 +5305,25 @@
         <v>20</v>
       </c>
       <c r="D14">
-        <v>4.6532745401</v>
+        <v>4.5772820532600003</v>
       </c>
       <c r="E14">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F14">
-        <v>0.94449381349100003</v>
+        <v>0.94484409285100002</v>
       </c>
       <c r="G14">
         <v>0.97727272727299996</v>
       </c>
       <c r="H14">
-        <v>0.90118577075100004</v>
+        <v>0.90909090909099999</v>
       </c>
       <c r="I14">
-        <v>0.46236559139799999</v>
+        <v>0.48314606741600002</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5319,25 +5337,25 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>15.6383667983</v>
+        <v>15.9619817951</v>
       </c>
       <c r="E15">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="F15">
-        <v>0.793522177228</v>
+        <v>0.78022953131299999</v>
       </c>
       <c r="G15">
         <v>0.63636363636399995</v>
       </c>
       <c r="H15">
-        <v>0.93675889328100004</v>
+        <v>0.889328063241</v>
       </c>
       <c r="I15">
-        <v>0.46666666666700002</v>
+        <v>0.33333333333300003</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5351,25 +5369,25 @@
         <v>20</v>
       </c>
       <c r="D16">
-        <v>0.30217889282400001</v>
+        <v>0.25390495012100001</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="F16">
-        <v>0.99704048822699998</v>
+        <v>0.99867041197700002</v>
       </c>
       <c r="G16">
-        <v>0.54166666666700003</v>
+        <v>0.625</v>
       </c>
       <c r="H16">
-        <v>0.96768060836500003</v>
+        <v>0.85551330798500003</v>
       </c>
       <c r="I16">
-        <v>0.433333333333</v>
+        <v>0.16483516483499999</v>
       </c>
       <c r="J16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5383,25 +5401,25 @@
         <v>20</v>
       </c>
       <c r="D17">
-        <v>3.72726504736</v>
+        <v>4.0546967159999996</v>
       </c>
       <c r="E17">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F17">
-        <v>0.85064292984000001</v>
+        <v>0.84242043688099999</v>
       </c>
       <c r="G17">
-        <v>0.5</v>
+        <v>0.54166666666700003</v>
       </c>
       <c r="H17">
-        <v>0.91444866920199996</v>
+        <v>0.89923954372600001</v>
       </c>
       <c r="I17">
-        <v>0.210526315789</v>
+        <v>0.19696969697</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5415,13 +5433,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>0.93329221339400004</v>
+        <v>2.00141657064</v>
       </c>
       <c r="E18">
         <v>550</v>
       </c>
       <c r="F18">
-        <v>0.99876079285599995</v>
+        <v>0.99721507880799998</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -5433,7 +5451,7 @@
         <v>0.08</v>
       </c>
       <c r="J18" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5447,13 +5465,13 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>20.146456748599999</v>
+        <v>13.2865290005</v>
       </c>
       <c r="E19">
         <v>550</v>
       </c>
       <c r="F19">
-        <v>0.74971456451100005</v>
+        <v>0.85926904874800003</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -5465,7 +5483,7 @@
         <v>0.08</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5479,13 +5497,13 @@
         <v>21</v>
       </c>
       <c r="D20">
-        <v>2.6519397060399998</v>
+        <v>2.70607684856</v>
       </c>
       <c r="E20">
         <v>550</v>
       </c>
       <c r="F20">
-        <v>0.86366972175199996</v>
+        <v>0.86276800140300003</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -5497,7 +5515,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5511,13 +5529,13 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>8.1861917765999994</v>
+        <v>8.0425591602799997</v>
       </c>
       <c r="E21">
         <v>550</v>
       </c>
       <c r="F21">
-        <v>0.68608206003899996</v>
+        <v>0.68123775520700003</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -5529,7 +5547,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5613,7 +5631,7 @@
         <v>0.109181141439</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5645,7 +5663,7 @@
         <v>0.12359550561800001</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5677,7 +5695,7 @@
         <v>7.5709779179799999E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5709,7 +5727,7 @@
         <v>6.70926517572E-2</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5723,13 +5741,13 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>628.06545560500001</v>
+        <v>344.430984244</v>
       </c>
       <c r="E6">
         <v>550</v>
       </c>
       <c r="F6">
-        <v>0.66857624268500004</v>
+        <v>0.58760368463799995</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -5755,13 +5773,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>224.68711120200001</v>
+        <v>132.271365008</v>
       </c>
       <c r="E7">
         <v>550</v>
       </c>
       <c r="F7">
-        <v>0.45698462269599999</v>
+        <v>0.46056804825199998</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -5773,7 +5791,7 @@
         <v>0.08</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5787,13 +5805,13 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>247.695633141</v>
+        <v>139.59971904400001</v>
       </c>
       <c r="E8">
         <v>550</v>
       </c>
       <c r="F8">
-        <v>0.53759075755700003</v>
+        <v>0.48500251585600002</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -5805,7 +5823,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5819,13 +5837,13 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>180.698173021</v>
+        <v>95.458197283499999</v>
       </c>
       <c r="E9">
         <v>550</v>
       </c>
       <c r="F9">
-        <v>0.43070704542400001</v>
+        <v>0.40716759877300002</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -5837,7 +5855,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5869,7 +5887,7 @@
         <v>0.19213973799100001</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5901,7 +5919,7 @@
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5933,7 +5951,7 @@
         <v>0.112676056338</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5965,7 +5983,7 @@
         <v>6.1662198391399997E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5997,7 +6015,7 @@
         <v>0.46236559139799999</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -6029,7 +6047,7 @@
         <v>0.33750000000000002</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -6061,7 +6079,7 @@
         <v>0.16483516483499999</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -6093,7 +6111,7 @@
         <v>0.19402985074599999</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6157,7 +6175,7 @@
         <v>0.08</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -6171,13 +6189,13 @@
         <v>21</v>
       </c>
       <c r="D20">
-        <v>2.6519397060399998</v>
+        <v>3.3304666763099999</v>
       </c>
       <c r="E20">
         <v>550</v>
       </c>
       <c r="F20">
-        <v>0.86366972175199996</v>
+        <v>0.85513146749699998</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -6189,7 +6207,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -6203,13 +6221,13 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>8.1469468881899996</v>
+        <v>8.2199576186099996</v>
       </c>
       <c r="E21">
         <v>550</v>
       </c>
       <c r="F21">
-        <v>0.67994035199799996</v>
+        <v>0.67922379697299995</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -6221,7 +6239,7 @@
         <v>4.36363636364E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotting tuning differences in summary
</commit_message>
<xml_diff>
--- a/python/results/tuning_summary.xlsx
+++ b/python/results/tuning_summary.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="134">
   <si>
     <t>setup</t>
   </si>
@@ -483,12 +483,63 @@
   </si>
   <si>
     <t>C=65.0</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Mean sensitivity</t>
+  </si>
+  <si>
+    <t>Mean specificity</t>
+  </si>
+  <si>
+    <t>Mean precision</t>
+  </si>
+  <si>
+    <t>Mean predictors</t>
+  </si>
+  <si>
+    <t>Tuning</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Predictor</t>
+  </si>
+  <si>
+    <t>Mean correlation</t>
+  </si>
+  <si>
+    <t>Correlation with true parameters</t>
+  </si>
+  <si>
+    <t>Correlation tuning</t>
+  </si>
+  <si>
+    <t>MSE tuning</t>
+  </si>
+  <si>
+    <t>Feature selection sensitivity</t>
+  </si>
+  <si>
+    <t>Feature selection specificity</t>
+  </si>
+  <si>
+    <t>Feature selection precision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -518,8 +569,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,6 +583,923 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Correlation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$B$36:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.88586138991200003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47042003372225005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88945332539824995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87439025467025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86421408121175003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correlation tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$C$36:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.85779847584275004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48524231708150001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87074520469374994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89154111825550009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85012247104149996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="85533056"/>
+        <c:axId val="85934080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85533056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85934080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85934080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85533056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sensitivity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$D$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$D$36:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.70643939393949995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70643939393924993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70643939393949995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$E$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correlation tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$E$36:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.83143939393924993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88446969696949995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69507575757600004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="69840896"/>
+        <c:axId val="69842432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69840896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69842432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69842432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69840896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Specificity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$F$36:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.88781767083975005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82149942139199994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88479688603675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$G$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correlation tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$G$36:$G$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.87920617983450011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80297832849875006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88829295601074998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="110391680"/>
+        <c:axId val="110394752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="110391680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110394752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="110394752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110391680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Precision</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$H$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$H$36:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.31414723114199999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1818181818200001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23016874372999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30005757663900001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1818181818200001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$I$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correlation tuning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$A$36:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>enet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gblasso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>grace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>lasso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$I$36:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.35889360500400003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1818181818200001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24385510973149999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2945710656385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1818181818200001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="102934016"/>
+        <c:axId val="102935936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="102934016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102935936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102935936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102934016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,13 +1811,1003 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(cv_mse_p550!D2:D5)</f>
+        <v>5.7488346817814993</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(cv_mse_p550!E2:E5)</f>
+        <v>75.5</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(cv_mse_p550!F2:F5)</f>
+        <v>0.89172156190925</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(cv_mse_p550!G2:G5)</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(cv_mse_p550!H2:H5)</f>
+        <v>0.90266422699475002</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(cv_mse_p550!I2:I5)</f>
+        <v>0.334852597202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" hidden="1">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(cv_mse_p550!D6:D9)</f>
+        <v>48.918005185825002</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE(cv_mse_p550!E6:E9)</f>
+        <v>550</v>
+      </c>
+      <c r="E5">
+        <f>AVERAGE(cv_mse_p550!F6:F9)</f>
+        <v>0.12016364245780002</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(cv_mse_p550!G6:G9)</f>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f>AVERAGE(cv_mse_p550!H6:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(cv_mse_p550!I6:I9)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(cv_mse_p550!D10:D13)</f>
+        <v>6.3917879115792493</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(cv_mse_p550!E10:E13)</f>
+        <v>73.5</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(cv_mse_p550!F10:F13)</f>
+        <v>0.8809496878680001</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(cv_mse_p550!G10:G13)</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(cv_mse_p550!H10:H13)</f>
+        <v>0.90680465591600001</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(cv_mse_p550!I10:I13)</f>
+        <v>0.36693577479875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="1">
+        <f>AVERAGE(cv_mse_p550!D14:D17)</f>
+        <v>5.8967247499285005</v>
+      </c>
+      <c r="D11" s="2">
+        <f>AVERAGE(cv_mse_p550!E14:E17)</f>
+        <v>83.25</v>
+      </c>
+      <c r="E11" s="1">
+        <f>AVERAGE(cv_mse_p550!F14:F17)</f>
+        <v>0.88586138991200003</v>
+      </c>
+      <c r="F11" s="1">
+        <f>AVERAGE(cv_mse_p550!G14:G17)</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="G11" s="1">
+        <f>AVERAGE(cv_mse_p550!H14:H17)</f>
+        <v>0.88781767083975005</v>
+      </c>
+      <c r="H11" s="1">
+        <f>AVERAGE(cv_mse_p550!I14:I17)</f>
+        <v>0.31414723114199999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="1">
+        <f>AVERAGE(coef_corr_p550!D2:D5)</f>
+        <v>7.3633839934675001</v>
+      </c>
+      <c r="D12" s="2">
+        <f>AVERAGE(coef_corr_p550!E2:E5)</f>
+        <v>90.75</v>
+      </c>
+      <c r="E12" s="1">
+        <f>AVERAGE(coef_corr_p550!F2:F5)</f>
+        <v>0.85779847584275004</v>
+      </c>
+      <c r="F12" s="1">
+        <f>AVERAGE(coef_corr_p550!G2:G5)</f>
+        <v>0.83143939393924993</v>
+      </c>
+      <c r="G12" s="1">
+        <f>AVERAGE(coef_corr_p550!H2:H5)</f>
+        <v>0.87920617983450011</v>
+      </c>
+      <c r="H12" s="1">
+        <f>AVERAGE(coef_corr_p550!I2:I5)</f>
+        <v>0.35889360500400003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(n_pred_p550!D2:D5)</f>
+        <v>53.922856935624999</v>
+      </c>
+      <c r="D13" s="2">
+        <f>AVERAGE(n_pred_p550!E2:E5)</f>
+        <v>347.25</v>
+      </c>
+      <c r="E13" s="1">
+        <f>AVERAGE(n_pred_p550!F2:F5)</f>
+        <v>0.6625158555945001</v>
+      </c>
+      <c r="F13" s="1">
+        <f>AVERAGE(n_pred_p550!G2:G5)</f>
+        <v>0.96875</v>
+      </c>
+      <c r="G13" s="1">
+        <f>AVERAGE(n_pred_p550!H2:H5)</f>
+        <v>0.39043643577450005</v>
+      </c>
+      <c r="H13" s="1">
+        <f>AVERAGE(n_pred_p550!I2:I5)</f>
+        <v>9.3894769498500008E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="1">
+        <f>AVERAGE(cv_mse_p550!D18:D21)</f>
+        <v>169.95507423437499</v>
+      </c>
+      <c r="D14" s="2">
+        <f>AVERAGE(cv_mse_p550!E18:E21)</f>
+        <v>550</v>
+      </c>
+      <c r="E14" s="1">
+        <f>AVERAGE(cv_mse_p550!F18:F21)</f>
+        <v>0.47042003372225005</v>
+      </c>
+      <c r="F14" s="1">
+        <f>AVERAGE(cv_mse_p550!G18:G21)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <f>AVERAGE(cv_mse_p550!H18:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f>AVERAGE(cv_mse_p550!I18:I21)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="1">
+        <f>AVERAGE(coef_corr_p550!D6:D9)</f>
+        <v>177.788443564375</v>
+      </c>
+      <c r="D15" s="2">
+        <f>AVERAGE(coef_corr_p550!E6:E9)</f>
+        <v>550</v>
+      </c>
+      <c r="E15" s="1">
+        <f>AVERAGE(coef_corr_p550!F6:F9)</f>
+        <v>0.48524231708150001</v>
+      </c>
+      <c r="F15" s="1">
+        <f>AVERAGE(coef_corr_p550!G6:G9)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <f>AVERAGE(coef_corr_p550!H6:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f>AVERAGE(coef_corr_p550!I6:I9)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="1">
+        <f>AVERAGE(n_pred_p550!D6:D9)</f>
+        <v>177.940066394875</v>
+      </c>
+      <c r="D16" s="2">
+        <f>AVERAGE(n_pred_p550!E6:E9)</f>
+        <v>550</v>
+      </c>
+      <c r="E16" s="1">
+        <f>AVERAGE(n_pred_p550!F6:F9)</f>
+        <v>0.48508546187974999</v>
+      </c>
+      <c r="F16" s="1">
+        <f>AVERAGE(n_pred_p550!G6:G9)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f>AVERAGE(n_pred_p550!H6:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>AVERAGE(n_pred_p550!I6:I9)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="1">
+        <f>AVERAGE(cv_mse_p550!D22:D25)</f>
+        <v>5.7922747426244996</v>
+      </c>
+      <c r="D17" s="2">
+        <f>AVERAGE(cv_mse_p550!E22:E25)</f>
+        <v>116.75</v>
+      </c>
+      <c r="E17" s="1">
+        <f>AVERAGE(cv_mse_p550!F22:F25)</f>
+        <v>0.88945332539824995</v>
+      </c>
+      <c r="F17" s="1">
+        <f>AVERAGE(cv_mse_p550!G22:G25)</f>
+        <v>0.70643939393924993</v>
+      </c>
+      <c r="G17" s="1">
+        <f>AVERAGE(cv_mse_p550!H22:H25)</f>
+        <v>0.82149942139199994</v>
+      </c>
+      <c r="H17" s="1">
+        <f>AVERAGE(cv_mse_p550!I22:I25)</f>
+        <v>0.23016874372999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="1">
+        <f>AVERAGE(coef_corr_p550!D10:D13)</f>
+        <v>5.9223832409872506</v>
+      </c>
+      <c r="D18" s="2">
+        <f>AVERAGE(coef_corr_p550!E10:E13)</f>
+        <v>132</v>
+      </c>
+      <c r="E18" s="1">
+        <f>AVERAGE(coef_corr_p550!F10:F13)</f>
+        <v>0.87074520469374994</v>
+      </c>
+      <c r="F18" s="1">
+        <f>AVERAGE(coef_corr_p550!G10:G13)</f>
+        <v>0.88446969696949995</v>
+      </c>
+      <c r="G18" s="1">
+        <f>AVERAGE(coef_corr_p550!H10:H13)</f>
+        <v>0.80297832849875006</v>
+      </c>
+      <c r="H18" s="1">
+        <f>AVERAGE(coef_corr_p550!I10:I13)</f>
+        <v>0.24385510973149999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="1">
+        <f>AVERAGE(n_pred_p550!D10:D13)</f>
+        <v>10.534569666128499</v>
+      </c>
+      <c r="D19" s="2">
+        <f>AVERAGE(n_pred_p550!E10:E13)</f>
+        <v>313.75</v>
+      </c>
+      <c r="E19" s="1">
+        <f>AVERAGE(n_pred_p550!F10:F13)</f>
+        <v>0.83202215920025013</v>
+      </c>
+      <c r="F19" s="1">
+        <f>AVERAGE(n_pred_p550!G10:G13)</f>
+        <v>0.98958333333324999</v>
+      </c>
+      <c r="G19" s="1">
+        <f>AVERAGE(n_pred_p550!H10:H13)</f>
+        <v>0.45676595680724996</v>
+      </c>
+      <c r="H19" s="1">
+        <f>AVERAGE(n_pred_p550!I10:I13)</f>
+        <v>0.11661949818010001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(cv_mse_p550!D26:D29)</f>
+        <v>6.6337139918219989</v>
+      </c>
+      <c r="D20" s="2">
+        <f>AVERAGE(cv_mse_p550!E26:E29)</f>
+        <v>84.75</v>
+      </c>
+      <c r="E20" s="1">
+        <f>AVERAGE(cv_mse_p550!F26:F29)</f>
+        <v>0.87439025467025</v>
+      </c>
+      <c r="F20" s="1">
+        <f>AVERAGE(cv_mse_p550!G26:G29)</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="G20" s="1">
+        <f>AVERAGE(cv_mse_p550!H26:H29)</f>
+        <v>0.88479688603675</v>
+      </c>
+      <c r="H20" s="1">
+        <f>AVERAGE(cv_mse_p550!I26:I29)</f>
+        <v>0.30005757663900001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="1">
+        <f>AVERAGE(coef_corr_p550!D14:D17)</f>
+        <v>6.2119663786202501</v>
+      </c>
+      <c r="D21" s="2">
+        <f>AVERAGE(coef_corr_p550!E14:E17)</f>
+        <v>82.5</v>
+      </c>
+      <c r="E21" s="1">
+        <f>AVERAGE(coef_corr_p550!F14:F17)</f>
+        <v>0.89154111825550009</v>
+      </c>
+      <c r="F21" s="1">
+        <f>AVERAGE(coef_corr_p550!G14:G17)</f>
+        <v>0.69507575757600004</v>
+      </c>
+      <c r="G21" s="1">
+        <f>AVERAGE(coef_corr_p550!H14:H17)</f>
+        <v>0.88829295601074998</v>
+      </c>
+      <c r="H21" s="1">
+        <f>AVERAGE(coef_corr_p550!I14:I17)</f>
+        <v>0.2945710656385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="1">
+        <f>AVERAGE(n_pred_p550!D14:D17)</f>
+        <v>6.2848452631002498</v>
+      </c>
+      <c r="D22" s="2">
+        <f>AVERAGE(n_pred_p550!E14:E17)</f>
+        <v>82.75</v>
+      </c>
+      <c r="E22" s="1">
+        <f>AVERAGE(n_pred_p550!F14:F17)</f>
+        <v>0.89064455890200001</v>
+      </c>
+      <c r="F22" s="1">
+        <f>AVERAGE(n_pred_p550!G14:G17)</f>
+        <v>0.68939393939400007</v>
+      </c>
+      <c r="G22" s="1">
+        <f>AVERAGE(n_pred_p550!H14:H17)</f>
+        <v>0.88732359969350005</v>
+      </c>
+      <c r="H22" s="1">
+        <f>AVERAGE(n_pred_p550!I14:I17)</f>
+        <v>0.28968265174474994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="1">
+        <f>AVERAGE(cv_mse_p550!D30:D33)</f>
+        <v>5.4820868909809999</v>
+      </c>
+      <c r="D23" s="2">
+        <f>AVERAGE(cv_mse_p550!E30:E33)</f>
+        <v>550</v>
+      </c>
+      <c r="E23" s="1">
+        <f>AVERAGE(cv_mse_p550!F30:F33)</f>
+        <v>0.86421408121175003</v>
+      </c>
+      <c r="F23" s="1">
+        <f>AVERAGE(cv_mse_p550!G30:G33)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <f>AVERAGE(cv_mse_p550!H30:H33)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f>AVERAGE(cv_mse_p550!I30:I33)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="1">
+        <f>AVERAGE(coef_corr_p550!D18:D21)</f>
+        <v>6.5091453949949996</v>
+      </c>
+      <c r="D24" s="2">
+        <f>AVERAGE(coef_corr_p550!E18:E21)</f>
+        <v>550</v>
+      </c>
+      <c r="E24" s="1">
+        <f>AVERAGE(coef_corr_p550!F18:F21)</f>
+        <v>0.85012247104149996</v>
+      </c>
+      <c r="F24" s="1">
+        <f>AVERAGE(coef_corr_p550!G18:G21)</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AVERAGE(coef_corr_p550!H18:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f>AVERAGE(coef_corr_p550!I18:I21)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="1">
+        <f>AVERAGE(n_pred_p550!D18:D21)</f>
+        <v>8.1575433142284997</v>
+      </c>
+      <c r="D25" s="2">
+        <f>AVERAGE(n_pred_p550!E18:E21)</f>
+        <v>550</v>
+      </c>
+      <c r="E25" s="1">
+        <f>AVERAGE(n_pred_p550!F18:F21)</f>
+        <v>0.82070765545924995</v>
+      </c>
+      <c r="F25" s="1">
+        <f>AVERAGE(n_pred_p550!G18:G21)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <f>AVERAGE(n_pred_p550!H18:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f>AVERAGE(n_pred_p550!I18:I21)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26">
+        <f>AVERAGE(cv_mse_p550!D34:D37)</f>
+        <v>81614.892315172503</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(cv_mse_p550!E34:E37)</f>
+        <v>550</v>
+      </c>
+      <c r="E26">
+        <f>AVERAGE(cv_mse_p550!F34:F37)</f>
+        <v>0.20172453232074999</v>
+      </c>
+      <c r="F26">
+        <f>AVERAGE(cv_mse_p550!G34:G37)</f>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>AVERAGE(cv_mse_p550!H34:H37)</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>AVERAGE(cv_mse_p550!I34:I37)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29">
+        <f>AVERAGE(cv_mse_p550!D38:D41)</f>
+        <v>15.824419772615002</v>
+      </c>
+      <c r="D29">
+        <f>AVERAGE(cv_mse_p550!E38:E41)</f>
+        <v>550</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(cv_mse_p550!F38:F41)</f>
+        <v>0.74404340699325</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(cv_mse_p550!G38:G41)</f>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f>AVERAGE(cv_mse_p550!H38:H41)</f>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f>AVERAGE(cv_mse_p550!I38:I41)</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="B34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="1">
+        <f>E11</f>
+        <v>0.88586138991200003</v>
+      </c>
+      <c r="C36" s="1">
+        <f>E12</f>
+        <v>0.85779847584275004</v>
+      </c>
+      <c r="D36" s="1">
+        <f>F11</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="E36" s="1">
+        <f>F12</f>
+        <v>0.83143939393924993</v>
+      </c>
+      <c r="F36" s="1">
+        <f>G11</f>
+        <v>0.88781767083975005</v>
+      </c>
+      <c r="G36" s="1">
+        <f>G12</f>
+        <v>0.87920617983450011</v>
+      </c>
+      <c r="H36" s="1">
+        <f>H11</f>
+        <v>0.31414723114199999</v>
+      </c>
+      <c r="I36" s="1">
+        <f>H12</f>
+        <v>0.35889360500400003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1">
+        <f>E14</f>
+        <v>0.47042003372225005</v>
+      </c>
+      <c r="C37" s="1">
+        <f>E15</f>
+        <v>0.48524231708150001</v>
+      </c>
+      <c r="D37" s="1">
+        <f>F14</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <f>F15</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <f>G14</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <f>G15</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <f>H14</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <f>H15</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1">
+        <f>E17</f>
+        <v>0.88945332539824995</v>
+      </c>
+      <c r="C38" s="1">
+        <f>E18</f>
+        <v>0.87074520469374994</v>
+      </c>
+      <c r="D38" s="1">
+        <f>F17</f>
+        <v>0.70643939393924993</v>
+      </c>
+      <c r="E38" s="1">
+        <f>F18</f>
+        <v>0.88446969696949995</v>
+      </c>
+      <c r="F38" s="1">
+        <f>G17</f>
+        <v>0.82149942139199994</v>
+      </c>
+      <c r="G38" s="1">
+        <f>G18</f>
+        <v>0.80297832849875006</v>
+      </c>
+      <c r="H38" s="1">
+        <f>H17</f>
+        <v>0.23016874372999999</v>
+      </c>
+      <c r="I38" s="1">
+        <f>H18</f>
+        <v>0.24385510973149999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="1">
+        <f>E20</f>
+        <v>0.87439025467025</v>
+      </c>
+      <c r="C39" s="1">
+        <f>E21</f>
+        <v>0.89154111825550009</v>
+      </c>
+      <c r="D39" s="1">
+        <f>F20</f>
+        <v>0.70643939393949995</v>
+      </c>
+      <c r="E39" s="1">
+        <f>F21</f>
+        <v>0.69507575757600004</v>
+      </c>
+      <c r="F39" s="1">
+        <f>G20</f>
+        <v>0.88479688603675</v>
+      </c>
+      <c r="G39" s="1">
+        <f>G21</f>
+        <v>0.88829295601074998</v>
+      </c>
+      <c r="H39" s="1">
+        <f>H20</f>
+        <v>0.30005757663900001</v>
+      </c>
+      <c r="I39" s="1">
+        <f>H21</f>
+        <v>0.2945710656385</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="1">
+        <f>E23</f>
+        <v>0.86421408121175003</v>
+      </c>
+      <c r="C40" s="1">
+        <f>E24</f>
+        <v>0.85012247104149996</v>
+      </c>
+      <c r="D40" s="1">
+        <f>F23</f>
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <f>F24</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <f>G23</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <f>G24</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <f>H23</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <f>H24</f>
+        <v>6.1818181818200001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -852,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2187,7 +4150,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3571,7 +5534,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:J6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Tuning summary minor changes
</commit_message>
<xml_diff>
--- a/python/results/tuning_summary.xlsx
+++ b/python/results/tuning_summary.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="136">
   <si>
     <t>setup</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Tuning</t>
   </si>
   <si>
-    <t>Correlation</t>
-  </si>
-  <si>
     <t>Predictor</t>
   </si>
   <si>
@@ -317,12 +314,6 @@
     <t>Correlation with true parameters</t>
   </si>
   <si>
-    <t>Correlation tuning</t>
-  </si>
-  <si>
-    <t>MSE tuning</t>
-  </si>
-  <si>
     <t>Feature selection sensitivity</t>
   </si>
   <si>
@@ -534,6 +525,18 @@
   </si>
   <si>
     <t>lambda 1=100.0, lambda 2=1000.0</t>
+  </si>
+  <si>
+    <t>CV MSE</t>
+  </si>
+  <si>
+    <t>CV MSE Tuning</t>
+  </si>
+  <si>
+    <t>Orchestra</t>
+  </si>
+  <si>
+    <t>Orchestra Tuning</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE tuning</c:v>
+                  <c:v>CV MSE Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -692,7 +695,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correlation tuning</c:v>
+                  <c:v>Orchestra Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -751,47 +754,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90621056"/>
-        <c:axId val="90622592"/>
+        <c:axId val="75548160"/>
+        <c:axId val="75549696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90621056"/>
+        <c:axId val="75548160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90622592"/>
+        <c:crossAx val="75549696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90622592"/>
+        <c:axId val="75549696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90621056"/>
+        <c:crossAx val="75548160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -833,7 +839,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE tuning</c:v>
+                  <c:v>CV MSE Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -901,7 +907,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correlation tuning</c:v>
+                  <c:v>Orchestra Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -960,47 +966,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90779008"/>
-        <c:axId val="90797184"/>
+        <c:axId val="144400384"/>
+        <c:axId val="144401920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90779008"/>
+        <c:axId val="144400384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90797184"/>
+        <c:crossAx val="144401920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90797184"/>
+        <c:axId val="144401920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90779008"/>
+        <c:crossAx val="144400384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1042,7 +1051,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE tuning</c:v>
+                  <c:v>CV MSE Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1110,7 +1119,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correlation tuning</c:v>
+                  <c:v>Orchestra Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1169,47 +1178,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90826240"/>
-        <c:axId val="90827776"/>
+        <c:axId val="144435072"/>
+        <c:axId val="144436608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90826240"/>
+        <c:axId val="144435072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90827776"/>
+        <c:crossAx val="144436608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90827776"/>
+        <c:axId val="144436608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90826240"/>
+        <c:crossAx val="144435072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1251,7 +1263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE tuning</c:v>
+                  <c:v>CV MSE Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1319,7 +1331,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correlation tuning</c:v>
+                  <c:v>Orchestra Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1378,47 +1390,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="160386432"/>
-        <c:axId val="160396416"/>
+        <c:axId val="144470016"/>
+        <c:axId val="144471552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="160386432"/>
+        <c:axId val="144470016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160396416"/>
+        <c:crossAx val="144471552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160396416"/>
+        <c:axId val="144471552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160386432"/>
+        <c:crossAx val="144470016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1460,7 +1475,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE tuning</c:v>
+                  <c:v>CV MSE Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1528,7 +1543,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correlation tuning</c:v>
+                  <c:v>Orchestra Tuning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1587,25 +1602,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="160433664"/>
-        <c:axId val="160435200"/>
+        <c:axId val="144508800"/>
+        <c:axId val="144510336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="160433664"/>
+        <c:axId val="144508800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160435200"/>
+        <c:crossAx val="144510336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160435200"/>
+        <c:axId val="144510336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,20 +1629,20 @@
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160433664"/>
+        <c:crossAx val="144508800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1668,15 +1683,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1697,16 +1712,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1228725</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1727,16 +1742,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2100,7 +2115,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2125,7 +2140,7 @@
         <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
         <v>53</v>
@@ -2142,7 +2157,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1">
         <f>AVERAGE(cv_mse_p550!D10:D13)</f>
@@ -2174,7 +2189,7 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1">
         <f>AVERAGE(coef_corr_p550!D2:D5)</f>
@@ -2206,7 +2221,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
         <f>AVERAGE(n_pred_p550!D2:D5)</f>
@@ -2238,7 +2253,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1">
         <f>AVERAGE(cv_mse_p550!D14:D17)</f>
@@ -2270,7 +2285,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1">
         <f>AVERAGE(coef_corr_p550!D6:D9)</f>
@@ -2302,7 +2317,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1">
         <f>AVERAGE(n_pred_p550!D6:D9)</f>
@@ -2334,7 +2349,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C8" s="1">
         <f>AVERAGE(cv_mse_p550!D18:D21)</f>
@@ -2366,7 +2381,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C9" s="1">
         <f>AVERAGE(coef_corr_p550!D10:D13)</f>
@@ -2398,7 +2413,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1">
         <f>AVERAGE(n_pred_p550!D10:D13)</f>
@@ -2430,7 +2445,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1">
         <f>AVERAGE(cv_mse_p550!D22:D24)</f>
@@ -2462,7 +2477,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C12" s="1">
         <f>AVERAGE(coef_corr_p550!D14:D17)</f>
@@ -2494,7 +2509,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
         <f>AVERAGE(n_pred_p550!D14:D17)</f>
@@ -2526,7 +2541,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1">
         <f>AVERAGE(cv_mse_p550!D10:D13)</f>
@@ -2558,7 +2573,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C15" s="1">
         <f>AVERAGE(coef_corr_p550!D18:D21)</f>
@@ -2590,7 +2605,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1">
         <f>AVERAGE(n_pred_p550!D18:D21)</f>
@@ -2622,7 +2637,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C17" s="1">
         <f>AVERAGE(cv_mse_p550!D14:D17)</f>
@@ -2654,7 +2669,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="C18" s="1">
         <f>AVERAGE(coef_corr_p550!D22:D25)</f>
@@ -2686,7 +2701,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1">
         <f>AVERAGE(n_pred_p550!D22:D25)</f>
@@ -2719,52 +2734,52 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11">
       <c r="B22" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="H22" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="K22" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -3108,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <v>1.3508563917900001</v>
@@ -3129,7 +3144,7 @@
         <v>0.56410256410299997</v>
       </c>
       <c r="J2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3140,7 +3155,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3">
         <v>16.412046992099999</v>
@@ -3161,7 +3176,7 @@
         <v>0.31868131868100003</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3172,7 +3187,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>0.19301668483600001</v>
@@ -3193,7 +3208,7 @@
         <v>0.3</v>
       </c>
       <c r="J4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3204,7 +3219,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5">
         <v>5.0394186583999998</v>
@@ -3225,7 +3240,7 @@
         <v>0.156626506024</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3257,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3289,7 +3304,7 @@
         <v>0.41509433962300002</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3321,7 +3336,7 @@
         <v>0.22857142857099999</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3353,7 +3368,7 @@
         <v>0.26373626373600001</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3385,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3417,7 +3432,7 @@
         <v>0.30136986301399998</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3449,7 +3464,7 @@
         <v>0.46875</v>
       </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3481,7 +3496,7 @@
         <v>0.16901408450700001</v>
       </c>
       <c r="J13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3513,7 +3528,7 @@
         <v>0.58666666666699996</v>
       </c>
       <c r="J14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3545,7 +3560,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3577,7 +3592,7 @@
         <v>0.245901639344</v>
       </c>
       <c r="J16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3609,7 +3624,7 @@
         <v>0.13402061855700001</v>
       </c>
       <c r="J17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3641,7 +3656,7 @@
         <v>0.12054794520500001</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3673,7 +3688,7 @@
         <v>9.5860566448800005E-2</v>
       </c>
       <c r="J19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3705,7 +3720,7 @@
         <v>4.6153846153799999E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3737,7 +3752,7 @@
         <v>5.0632911392399997E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3769,7 +3784,7 @@
         <v>0.196428571429</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3801,7 +3816,7 @@
         <v>0.31868131868100003</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3833,7 +3848,7 @@
         <v>0.26415094339599998</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3865,7 +3880,7 @@
         <v>0.14141414141399999</v>
       </c>
       <c r="J25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -4121,7 +4136,7 @@
         <v>0.26373626373600001</v>
       </c>
       <c r="J33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -4153,7 +4168,7 @@
         <v>9.5238095238100007E-2</v>
       </c>
       <c r="J34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -4185,7 +4200,7 @@
         <v>9.2243186582799994E-2</v>
       </c>
       <c r="J35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4217,7 +4232,7 @@
         <v>0.18604651162800001</v>
       </c>
       <c r="J36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4249,7 +4264,7 @@
         <v>0.14117647058800001</v>
       </c>
       <c r="J37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4281,7 +4296,7 @@
         <v>0.323529411765</v>
       </c>
       <c r="J38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4313,7 +4328,7 @@
         <v>0.08</v>
       </c>
       <c r="J39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4345,7 +4360,7 @@
         <v>0.25423728813599999</v>
       </c>
       <c r="J40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -4377,7 +4392,7 @@
         <v>8.984375E-2</v>
       </c>
       <c r="J41" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -4462,7 +4477,7 @@
         <v>0.57142857142900005</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4494,7 +4509,7 @@
         <v>0.35632183907999998</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4526,7 +4541,7 @@
         <v>0.35384615384599999</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4558,7 +4573,7 @@
         <v>0.12258064516099999</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4590,7 +4605,7 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4622,7 +4637,7 @@
         <v>0.63043478260899999</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4654,7 +4669,7 @@
         <v>0.56666666666700005</v>
       </c>
       <c r="J8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4686,7 +4701,7 @@
         <v>0.16</v>
       </c>
       <c r="J9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4718,7 +4733,7 @@
         <v>0.12054794520500001</v>
       </c>
       <c r="J10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4750,7 +4765,7 @@
         <v>9.5860566448800005E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -4782,7 +4797,7 @@
         <v>4.6153846153799999E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -4814,7 +4829,7 @@
         <v>4.6783625730999999E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -4878,7 +4893,7 @@
         <v>0.30392156862699998</v>
       </c>
       <c r="J15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -4910,7 +4925,7 @@
         <v>0.56097560975600003</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -4942,7 +4957,7 @@
         <v>0.13768115942</v>
       </c>
       <c r="J17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4974,7 +4989,7 @@
         <v>0.48314606741600002</v>
       </c>
       <c r="J18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5006,7 +5021,7 @@
         <v>0.32558139534899999</v>
       </c>
       <c r="J19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5038,7 +5053,7 @@
         <v>0.26415094339599998</v>
       </c>
       <c r="J20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5070,7 +5085,7 @@
         <v>0.19696969697</v>
       </c>
       <c r="J21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5283,7 +5298,7 @@
         <v>0.108374384236</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5315,7 +5330,7 @@
         <v>0.36904761904799999</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5347,7 +5362,7 @@
         <v>0.15</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5379,7 +5394,7 @@
         <v>0.125</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5411,7 +5426,7 @@
         <v>0.109452736318</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5443,7 +5458,7 @@
         <v>0.59574468085099996</v>
       </c>
       <c r="J7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5475,7 +5490,7 @@
         <v>0.14371257485</v>
       </c>
       <c r="J8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5507,7 +5522,7 @@
         <v>7.07395498392E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5539,7 +5554,7 @@
         <v>8.2089552238800004E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5571,7 +5586,7 @@
         <v>0.117962466488</v>
       </c>
       <c r="J11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5603,7 +5618,7 @@
         <v>0.12903225806499999</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5699,7 +5714,7 @@
         <v>0.30392156862699998</v>
       </c>
       <c r="J15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5763,7 +5778,7 @@
         <v>0.14285714285699999</v>
       </c>
       <c r="J17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6084,7 +6099,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <v>1.92342303886</v>
@@ -6105,7 +6120,7 @@
         <v>0.63768115942000003</v>
       </c>
       <c r="J2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6116,7 +6131,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3">
         <v>14.612980673999999</v>
@@ -6137,7 +6152,7 @@
         <v>0.448275862069</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6148,7 +6163,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>0.77870490857399999</v>
@@ -6169,7 +6184,7 @@
         <v>0.28301886792499997</v>
       </c>
       <c r="J4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6180,7 +6195,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5">
         <v>4.3964644269199997</v>
@@ -6201,7 +6216,7 @@
         <v>0.26388888888899997</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6233,7 +6248,7 @@
         <v>0.95652173913000005</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -6265,7 +6280,7 @@
         <v>0.511627906977</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -6311,7 +6326,7 @@
         <v>0.222222222222</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -6343,7 +6358,7 @@
         <v>0.97777777777800001</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -6375,7 +6390,7 @@
         <v>0.48888888888900001</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -6407,7 +6422,7 @@
         <v>0.29411764705900001</v>
       </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -6439,7 +6454,7 @@
         <v>0.260273972603</v>
       </c>
       <c r="J13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -6471,7 +6486,7 @@
         <v>0.62857142857100001</v>
       </c>
       <c r="J14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -6503,7 +6518,7 @@
         <v>0.39583333333300003</v>
       </c>
       <c r="J15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -6535,7 +6550,7 @@
         <v>0.26315789473700002</v>
       </c>
       <c r="J16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -6567,7 +6582,7 @@
         <v>0.22471910112400001</v>
       </c>
       <c r="J17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6599,7 +6614,7 @@
         <v>0.51764705882399997</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -6631,7 +6646,7 @@
         <v>0.48351648351600002</v>
       </c>
       <c r="J19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -6663,7 +6678,7 @@
         <v>0.252631578947</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -6695,7 +6710,7 @@
         <v>0.24</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -6727,7 +6742,7 @@
         <v>0.29139072847699998</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -6759,7 +6774,7 @@
         <v>0.37623762376199998</v>
       </c>
       <c r="J23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -6791,7 +6806,7 @@
         <v>0.28846153846200001</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6823,7 +6838,7 @@
         <v>0.26760563380300001</v>
       </c>
       <c r="J25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7175,7 +7190,7 @@
         <v>0.23529411764700001</v>
       </c>
       <c r="J36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -7207,7 +7222,7 @@
         <v>0.222222222222</v>
       </c>
       <c r="J37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -7239,7 +7254,7 @@
         <v>0.4</v>
       </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -7271,7 +7286,7 @@
         <v>0.61111111111100003</v>
       </c>
       <c r="J39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -7303,7 +7318,7 @@
         <v>0.25423728813599999</v>
       </c>
       <c r="J40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -7335,7 +7350,7 @@
         <v>0.218390804598</v>
       </c>
       <c r="J41" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -7418,7 +7433,7 @@
         <v>0.56410256410299997</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -7450,7 +7465,7 @@
         <v>0.57352941176500005</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -7482,7 +7497,7 @@
         <v>0.255319148936</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7514,7 +7529,7 @@
         <v>0.316666666667</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7546,7 +7561,7 @@
         <v>0.51764705882399997</v>
       </c>
       <c r="J6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7578,7 +7593,7 @@
         <v>0.78947368421099995</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -7610,7 +7625,7 @@
         <v>0.51428571428600001</v>
       </c>
       <c r="J8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -7642,7 +7657,7 @@
         <v>0.29032258064499999</v>
       </c>
       <c r="J9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -7674,7 +7689,7 @@
         <v>0.51764705882399997</v>
       </c>
       <c r="J10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -7706,7 +7721,7 @@
         <v>0.48351648351600002</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7770,7 +7785,7 @@
         <v>0.24</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7802,7 +7817,7 @@
         <v>0.60273972602699999</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7834,7 +7849,7 @@
         <v>0.387755102041</v>
       </c>
       <c r="J15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -7866,7 +7881,7 @@
         <v>0.59459459459499997</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7898,7 +7913,7 @@
         <v>0.54838709677399999</v>
       </c>
       <c r="J17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7930,7 +7945,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7962,7 +7977,7 @@
         <v>0.458823529412</v>
       </c>
       <c r="J19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -8026,7 +8041,7 @@
         <v>0.33333333333300003</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8237,7 +8252,7 @@
         <v>0.63768115942000003</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -8269,7 +8284,7 @@
         <v>0.53658536585399996</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -8301,7 +8316,7 @@
         <v>0.47058823529400001</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -8333,7 +8348,7 @@
         <v>0.375</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8365,7 +8380,7 @@
         <v>0.37606837606799998</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -8397,7 +8412,7 @@
         <v>0.30399999999999999</v>
       </c>
       <c r="J7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -8429,7 +8444,7 @@
         <v>0.29268292682899999</v>
       </c>
       <c r="J8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8461,7 +8476,7 @@
         <v>0.141935483871</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -8481,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -8525,7 +8540,7 @@
         <v>0.48351648351600002</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -8557,7 +8572,7 @@
         <v>0.52173913043499998</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -8589,7 +8604,7 @@
         <v>0.56410256410299997</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -8621,7 +8636,7 @@
         <v>0.62857142857100001</v>
       </c>
       <c r="J14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -8653,7 +8668,7 @@
         <v>0.43564356435599999</v>
       </c>
       <c r="J15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -8685,7 +8700,7 @@
         <v>0.328125</v>
       </c>
       <c r="J16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -8717,7 +8732,7 @@
         <v>0.26250000000000001</v>
       </c>
       <c r="J17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -8749,7 +8764,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -8781,7 +8796,7 @@
         <v>0.46428571428600002</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -8973,7 +8988,7 @@
         <v>0.29268292682899999</v>
       </c>
       <c r="J25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>